<commit_message>
These are my changes to the homework files
</commit_message>
<xml_diff>
--- a/Assignments/ChartBuilder/Exercise1/Chartbuilder1.xlsx
+++ b/Assignments/ChartBuilder/Exercise1/Chartbuilder1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-30000" yWindow="280" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t>State</t>
   </si>
@@ -216,7 +216,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,16 +272,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -309,6 +322,13 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -336,6 +356,13 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -667,7 +694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1891,201 +1920,428 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1">
+        <v>34</v>
+      </c>
+      <c r="C2" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>106</v>
+      </c>
+      <c r="C5" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>102</v>
+      </c>
+      <c r="C7" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>58</v>
+      </c>
+      <c r="C11" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43</v>
+      </c>
+      <c r="C16" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>17</v>
+      </c>
+      <c r="C17" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>24</v>
+      </c>
+      <c r="C21" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>40</v>
+      </c>
+      <c r="C22" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>12</v>
+      </c>
+      <c r="C23" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>52</v>
+      </c>
+      <c r="C25" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>46</v>
+      </c>
+      <c r="C26" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>53</v>
+      </c>
+      <c r="C27" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>56</v>
+      </c>
+      <c r="C28" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>26</v>
+      </c>
+      <c r="C29" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>32</v>
+      </c>
+      <c r="C30" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>59</v>
+      </c>
+      <c r="C31" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>54</v>
+      </c>
+      <c r="C32" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>82</v>
+      </c>
+      <c r="C33" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>47</v>
+      </c>
+      <c r="C34" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>97</v>
+      </c>
+      <c r="C35" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>12</v>
+      </c>
+      <c r="C36" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>16</v>
+      </c>
+      <c r="C37" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="C40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>